<commit_message>
Corrige caminho absoluto da base de dados
</commit_message>
<xml_diff>
--- a/data/Base_de_notas.xlsx
+++ b/data/Base_de_notas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://videomar-my.sharepoint.com/personal/joao_miranda_alaresinternet_com_br/Documents/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://videomar-my.sharepoint.com/personal/joao_miranda_alaresinternet_com_br/Documents/Área de Trabalho/Projeto-Recebimento-de-Notas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_AD4D361C20488DEA4E38A009645944A25ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB9D19FB-3665-41B5-9A38-1425E6496645}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_AD4D361C20488DEA4E38A009645944A25ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{425D43B3-EF99-4C2A-B783-596DA333A327}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>UF</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>27302</t>
-  </si>
-  <si>
-    <t>72000</t>
   </si>
   <si>
     <t>99623</t>
@@ -434,7 +431,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +450,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -467,7 +464,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -477,11 +474,11 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="C3">
+        <v>72000</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,10 +489,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -506,10 +503,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -517,13 +514,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,13 +528,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,41 +542,41 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,13 +584,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>